<commit_message>
enable git vscode setting file
</commit_message>
<xml_diff>
--- a/test/B 參數.xlsx
+++ b/test/B 參數.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\學評組工讀生\應數碩三_陳慎逸\程式學習\Index-Evaluation-Analysis-Report\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956141B5-5D5B-43A9-A1BD-6D945D32DCB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F561DFA-D253-430F-BE4E-77A3B055FD4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="參數" sheetId="5" r:id="rId1"/>
-    <sheet name="評鑑指標" sheetId="1" r:id="rId2"/>
-    <sheet name="科系列表" sheetId="3" r:id="rId3"/>
+    <sheet name="評鑑指標" sheetId="1" r:id="rId1"/>
+    <sheet name="科系列表" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="376">
   <si>
     <t>編號</t>
   </si>
@@ -1147,10 +1146,6 @@
   </si>
   <si>
     <t>7A0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>本次指標學年度</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1212,7 +1207,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1257,13 +1252,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="標楷體"/>
-      <family val="4"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="標楷體"/>
       <family val="4"/>
@@ -1359,7 +1347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1473,9 +1461,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2155,44 +2140,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE9EF79C-B6DC-4966-8323-52D8F19EFDAE}">
-  <sheetPr codeName="工作表1"/>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="41" t="s">
-        <v>362</v>
-      </c>
-      <c r="B1" s="39">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="40"/>
-      <c r="B3" s="40"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="工作表2"/>
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
@@ -3563,12 +3515,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C6F4F1D-4402-498D-B742-AC62FD83CA7B}">
   <sheetPr codeName="工作表4"/>
   <dimension ref="A1:D107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
@@ -3596,13 +3548,13 @@
     </row>
     <row r="2" spans="1:4" ht="16.5">
       <c r="A2" s="30" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>351</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D2" s="31" t="s">
         <v>352</v>
@@ -3610,7 +3562,7 @@
     </row>
     <row r="3" spans="1:4" ht="16.5">
       <c r="A3" s="30" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B3" s="32">
         <v>100</v>
@@ -3619,12 +3571,12 @@
         <v>177</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.5">
       <c r="A4" s="30" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B4" s="36">
         <v>700</v>
@@ -3633,12 +3585,12 @@
         <v>199</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16.5">
       <c r="A5" s="30" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B5" s="31">
         <v>200</v>
@@ -3647,12 +3599,12 @@
         <v>208</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.5">
       <c r="A6" s="30" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B6" s="31">
         <v>600</v>
@@ -3661,12 +3613,12 @@
         <v>241</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16.5">
       <c r="A7" s="30" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B7" s="31">
         <v>300</v>
@@ -3675,12 +3627,12 @@
         <v>248</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16.5">
       <c r="A8" s="30" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B8" s="31">
         <v>500</v>
@@ -3689,12 +3641,12 @@
         <v>273</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16.5">
       <c r="A9" s="30" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B9" s="31">
         <v>400</v>
@@ -3703,12 +3655,12 @@
         <v>296</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16.5">
       <c r="A10" s="30" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B10" s="31">
         <v>800</v>
@@ -3717,12 +3669,12 @@
         <v>314</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16.5">
       <c r="A11" s="30" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B11" s="31">
         <v>900</v>
@@ -3731,35 +3683,35 @@
         <v>331</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16.5">
       <c r="A12" s="30" t="s">
+        <v>362</v>
+      </c>
+      <c r="B12" s="31" t="s">
         <v>363</v>
-      </c>
-      <c r="B12" s="31" t="s">
-        <v>364</v>
       </c>
       <c r="C12" s="30" t="s">
         <v>341</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16.5">
       <c r="A13" s="30" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C13" s="30" t="s">
         <v>346</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16.5">
@@ -3786,7 +3738,7 @@
       <c r="C15" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="39" t="s">
         <v>179</v>
       </c>
     </row>
@@ -3800,7 +3752,7 @@
       <c r="C16" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="39" t="s">
         <v>181</v>
       </c>
     </row>
@@ -3814,7 +3766,7 @@
       <c r="C17" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="D17" s="42" t="s">
+      <c r="D17" s="39" t="s">
         <v>182</v>
       </c>
     </row>
@@ -3828,7 +3780,7 @@
       <c r="C18" s="35" t="s">
         <v>183</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="39" t="s">
         <v>184</v>
       </c>
     </row>
@@ -3842,7 +3794,7 @@
       <c r="C19" s="35" t="s">
         <v>185</v>
       </c>
-      <c r="D19" s="42" t="s">
+      <c r="D19" s="39" t="s">
         <v>186</v>
       </c>
     </row>
@@ -3856,7 +3808,7 @@
       <c r="C20" s="35" t="s">
         <v>187</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="39" t="s">
         <v>188</v>
       </c>
     </row>
@@ -3870,7 +3822,7 @@
       <c r="C21" s="35" t="s">
         <v>189</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="39" t="s">
         <v>190</v>
       </c>
     </row>
@@ -3884,7 +3836,7 @@
       <c r="C22" s="35" t="s">
         <v>191</v>
       </c>
-      <c r="D22" s="42" t="s">
+      <c r="D22" s="39" t="s">
         <v>192</v>
       </c>
     </row>

</xml_diff>